<commit_message>
Added annotation to make code easier to understand
</commit_message>
<xml_diff>
--- a/_Modafinil/Route_3.xlsx
+++ b/_Modafinil/Route_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mseifrid/Dropbox (Aspuru-Guzik Lab)/Matter Lab/Data/Code/Chemical subway/RouteScore_preprint/modafinil/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mseifrid/Dropbox (Aspuru-Guzik Lab)/Matter Lab/Data/Code/Subway_Maps/_Modafinil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5560E14-7FB4-6049-851B-9CB90C6A013A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5D3A8C-F559-AA40-8C54-E8488FBBD200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{662B73D7-7059-1B4C-85E4-D7993B3B5A7C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="2" xr2:uid="{662B73D7-7059-1B4C-85E4-D7993B3B5A7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1" sheetId="1" r:id="rId1"/>
@@ -167,15 +167,6 @@
     <t>7.9 g</t>
   </si>
   <si>
-    <t>3M methanolic ammonia solution</t>
-  </si>
-  <si>
-    <t>[NH4+].[OH-]</t>
-  </si>
-  <si>
-    <t>https://www.fishersci.com/shop/products/ammonium-hydroxide-solution-3m/S25844</t>
-  </si>
-  <si>
     <t>50 mL</t>
   </si>
   <si>
@@ -183,6 +174,15 @@
   </si>
   <si>
     <t>50 mg</t>
+  </si>
+  <si>
+    <t>ammonia</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>https://www.sigmaaldrich.com/catalog/product/aldrich/294993?lang=en&amp;region=CA</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A113539-C27A-474D-AB54-C3F8D13988D2}">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
@@ -771,7 +771,7 @@
         <v>4.5454545450000002E-5</v>
       </c>
       <c r="I4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
@@ -950,7 +950,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E220EEC7-C513-E645-8D34-F7421F6092A9}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,11 +1125,11 @@
       </c>
       <c r="S2">
         <f>SUM(K2:K12)+N2*O2</f>
-        <v>80.23</v>
+        <v>91.896917647058828</v>
       </c>
       <c r="T2">
         <f>SUM(L2:L12)</f>
-        <v>13.245072</v>
+        <v>10.542072000000001</v>
       </c>
       <c r="V2" t="s">
         <v>32</v>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="X2">
         <f>S2/Y2</f>
-        <v>3666.3163186034826</v>
+        <v>4199.4661448182987</v>
       </c>
       <c r="Y2">
         <f>P2*MIN(H2:H6)</f>
@@ -1147,50 +1147,50 @@
       </c>
       <c r="Z2">
         <f>R2*S2*T2</f>
-        <v>1593.9781898400001</v>
+        <v>1453.1758836200472</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3">
-        <v>35.049999999999997</v>
+        <v>17.03</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E3">
-        <v>7.75</v>
+        <v>828</v>
       </c>
       <c r="F3">
-        <v>52.575000000000003</v>
+        <v>170</v>
       </c>
       <c r="G3">
         <f>E3/(F3/C3)</f>
-        <v>5.1666666666666661</v>
+        <v>82.946117647058827</v>
       </c>
       <c r="H3">
         <v>0.15</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3" si="0">H3*G3</f>
-        <v>0.77499999999999991</v>
+        <v>12.441917647058824</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3" si="1">H3*C3</f>
-        <v>5.2574999999999994</v>
+        <v>2.5545</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{12B52D6D-A79F-9E44-9392-C07CB13A5BC2}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{802C8B39-80E7-3B4C-9C16-545C0BA5BF62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>